<commit_message>
experiments now done for all users, commiting before trying: checking how many times each algorithm can track arm change.
</commit_message>
<xml_diff>
--- a/stationarity_test/KLDivergenceTest/FeedbackLog/p2-faa-0ms.xlsx
+++ b/stationarity_test/KLDivergenceTest/FeedbackLog/p2-faa-0ms.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\imMens Learning\stationarity_test\KLDivergenceTest\FeedbackLog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanadsaha92/Desktop/Research_Experiments/imMens-Interactions/stationarity_test/KLDivergenceTest/FeedbackLog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5692FF-2BC6-4FB5-A1FC-CA1E2FE3A41B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74E6D0C-16E7-1C4D-B019-991240236743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -653,7 +653,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -671,15 +671,15 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="3"/>
-    <col min="10" max="10" width="38.85546875" customWidth="1"/>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="3"/>
+    <col min="10" max="10" width="38.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -708,7 +708,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -737,7 +737,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -763,7 +763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -789,7 +789,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -815,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -844,7 +844,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -870,7 +870,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -896,7 +896,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -922,7 +922,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -948,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -974,7 +974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -998,7 +998,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -1206,7 +1206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -1336,7 +1336,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -1388,7 +1388,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
@@ -1414,7 +1414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="42" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -1521,7 +1521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -1599,7 +1599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="56" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="42" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
@@ -1657,7 +1657,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>54</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
@@ -1761,7 +1761,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>56</v>
       </c>
@@ -1787,7 +1787,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
@@ -1816,7 +1816,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>59</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>60</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>61</v>
       </c>
@@ -1912,15 +1912,15 @@
       <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" style="3"/>
-    <col min="11" max="11" width="38.85546875" customWidth="1"/>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" style="3"/>
+    <col min="11" max="11" width="38.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -1984,7 +1984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -2013,7 +2013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -2042,7 +2042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -2103,7 +2103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -2248,7 +2248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -2277,7 +2277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -2509,7 +2509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -2538,7 +2538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -2567,7 +2567,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -2596,7 +2596,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -2654,7 +2654,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -2712,7 +2712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
@@ -2741,7 +2741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
@@ -2770,7 +2770,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -2799,7 +2799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="42" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -2918,7 +2918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="51" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="56" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="42" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>50</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>52</v>
       </c>
@@ -3040,7 +3040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>53</v>
       </c>
@@ -3069,7 +3069,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>54</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>55</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="28" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>56</v>
       </c>
@@ -3156,7 +3156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="28" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>57</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>59</v>
       </c>
@@ -3217,7 +3217,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A45" s="1" t="s">
         <v>60</v>
       </c>
@@ -3246,7 +3246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="14" x14ac:dyDescent="0.15">
       <c r="A46" s="1" t="s">
         <v>61</v>
       </c>
@@ -3289,18 +3289,18 @@
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="6" max="7" width="17.28515625" style="6"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="6"/>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="6" max="7" width="17.33203125" style="6"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3328,7 +3328,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -3356,7 +3356,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -3384,7 +3384,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -3412,7 +3412,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -3440,7 +3440,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -3468,7 +3468,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -3496,7 +3496,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -3524,7 +3524,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -3552,7 +3552,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -3580,7 +3580,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -3608,7 +3608,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -3636,7 +3636,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -3664,7 +3664,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -3692,7 +3692,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -3720,7 +3720,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -3748,7 +3748,7 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
@@ -3776,7 +3776,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -3804,7 +3804,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -3832,7 +3832,7 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -3860,7 +3860,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -3888,7 +3888,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -3916,7 +3916,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -3944,7 +3944,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -3972,7 +3972,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -4000,7 +4000,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -4028,7 +4028,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -4056,7 +4056,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
@@ -4084,7 +4084,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
@@ -4112,7 +4112,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -4140,7 +4140,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -4168,7 +4168,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -4196,7 +4196,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -4224,7 +4224,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -4252,7 +4252,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -4280,7 +4280,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -4308,7 +4308,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>52</v>
       </c>
@@ -4336,7 +4336,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>53</v>
       </c>
@@ -4364,7 +4364,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>54</v>
       </c>
@@ -4392,7 +4392,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
@@ -4420,7 +4420,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>57</v>
       </c>
@@ -4448,7 +4448,7 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>59</v>
       </c>
@@ -4476,7 +4476,7 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
@@ -4504,7 +4504,7 @@
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>61</v>
       </c>
@@ -4541,23 +4541,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{578BA753-ECCC-462E-92EB-30D03CB00AD3}">
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="89" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="70.7109375" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" style="6"/>
-    <col min="7" max="7" width="19.42578125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="6" customWidth="1"/>
-    <col min="10" max="10" width="9.140625" style="6"/>
+    <col min="1" max="1" width="70.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" style="6"/>
+    <col min="7" max="7" width="19.5" style="6" customWidth="1"/>
+    <col min="8" max="8" width="23.33203125" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4585,7 +4585,7 @@
       <c r="I1" s="5"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -4613,7 +4613,7 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
-    <row r="3" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -4641,7 +4641,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -4669,7 +4669,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -4697,7 +4697,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -4725,7 +4725,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -4753,7 +4753,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
@@ -4781,7 +4781,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -4809,7 +4809,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -4837,7 +4837,7 @@
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -4865,7 +4865,7 @@
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A12" s="1" t="s">
         <v>21</v>
       </c>
@@ -4893,7 +4893,7 @@
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A13" s="1" t="s">
         <v>22</v>
       </c>
@@ -4921,7 +4921,7 @@
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A14" s="1" t="s">
         <v>23</v>
       </c>
@@ -4949,7 +4949,7 @@
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A15" s="1" t="s">
         <v>24</v>
       </c>
@@ -4977,7 +4977,7 @@
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A16" s="1" t="s">
         <v>25</v>
       </c>
@@ -5005,12 +5005,12 @@
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B17" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>74</v>
@@ -5033,7 +5033,7 @@
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A18" s="1" t="s">
         <v>27</v>
       </c>
@@ -5061,7 +5061,7 @@
       <c r="I18" s="5"/>
       <c r="J18" s="5"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A19" s="1" t="s">
         <v>28</v>
       </c>
@@ -5089,12 +5089,12 @@
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B20" s="4">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>70</v>
@@ -5117,7 +5117,7 @@
       <c r="I20" s="5"/>
       <c r="J20" s="5"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A21" s="1" t="s">
         <v>30</v>
       </c>
@@ -5145,7 +5145,7 @@
       <c r="I21" s="5"/>
       <c r="J21" s="5"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A22" s="1" t="s">
         <v>32</v>
       </c>
@@ -5173,7 +5173,7 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
@@ -5201,7 +5201,7 @@
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -5229,7 +5229,7 @@
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A25" s="1" t="s">
         <v>35</v>
       </c>
@@ -5257,7 +5257,7 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -5285,7 +5285,7 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -5313,7 +5313,7 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
@@ -5341,7 +5341,7 @@
       <c r="I28" s="5"/>
       <c r="J28" s="5"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
@@ -5369,7 +5369,7 @@
       <c r="I29" s="5"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -5397,7 +5397,7 @@
       <c r="I30" s="5"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A31" s="1" t="s">
         <v>42</v>
       </c>
@@ -5425,7 +5425,7 @@
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -5453,7 +5453,7 @@
       <c r="I32" s="5"/>
       <c r="J32" s="5"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A33" s="1" t="s">
         <v>45</v>
       </c>
@@ -5481,7 +5481,7 @@
       <c r="I33" s="5"/>
       <c r="J33" s="5"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -5509,7 +5509,7 @@
       <c r="I34" s="5"/>
       <c r="J34" s="5"/>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A35" s="1" t="s">
         <v>47</v>
       </c>
@@ -5537,7 +5537,7 @@
       <c r="I35" s="5"/>
       <c r="J35" s="5"/>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A36" s="1" t="s">
         <v>48</v>
       </c>
@@ -5565,7 +5565,7 @@
       <c r="I36" s="5"/>
       <c r="J36" s="5"/>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A37" s="1" t="s">
         <v>52</v>
       </c>
@@ -5593,7 +5593,7 @@
       <c r="I37" s="5"/>
       <c r="J37" s="5"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A38" s="1" t="s">
         <v>53</v>
       </c>
@@ -5621,7 +5621,7 @@
       <c r="I38" s="5"/>
       <c r="J38" s="5"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A39" s="1" t="s">
         <v>54</v>
       </c>
@@ -5649,7 +5649,7 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A40" s="1" t="s">
         <v>55</v>
       </c>
@@ -5677,7 +5677,7 @@
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
-    <row r="41" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:10" ht="28" x14ac:dyDescent="0.15">
       <c r="A41" s="1" t="s">
         <v>57</v>
       </c>
@@ -5705,7 +5705,7 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A42" s="1" t="s">
         <v>59</v>
       </c>
@@ -5733,7 +5733,7 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A43" s="1" t="s">
         <v>60</v>
       </c>
@@ -5761,7 +5761,7 @@
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="14" x14ac:dyDescent="0.15">
       <c r="A44" s="1" t="s">
         <v>61</v>
       </c>

</xml_diff>